<commit_message>
update for house auction apply for approval
</commit_message>
<xml_diff>
--- a/static/template_error.xlsx
+++ b/static/template_error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i300822/Desktop/Meebid Git/MeebidUI/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37247DBB-8F50-F545-B03C-0635942210AF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94EF343-338B-AD4F-927F-66123DB7CFE0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="460" windowWidth="28140" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>